<commit_message>
criacao das classes RegisterPage, RegisterStep, RegisterLogic, RegisterRunner e da feature register.feature
</commit_message>
<xml_diff>
--- a/Usuario_Cadastro.xlsx
+++ b/Usuario_Cadastro.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\eclipse-workspace\advantage-shopping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C02212E1-D919-41B5-9B6D-5099921C40F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CB0997-2497-4452-A09A-500F8D5D05A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{B6BE7F0E-3B9E-4F50-8BA9-7697DEB93021}"/>
   </bookViews>
@@ -37,42 +37,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
-    <t>User</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>First_Name</t>
-  </si>
-  <si>
-    <t>Last_Name</t>
-  </si>
-  <si>
-    <t>Telephone</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Adress</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Zip_Code</t>
-  </si>
-  <si>
-    <t>gabrieloms</t>
-  </si>
-  <si>
     <t>gabriel@keeggo.com</t>
   </si>
   <si>
@@ -101,13 +68,46 @@
   </si>
   <si>
     <t>08130-310</t>
+  </si>
+  <si>
+    <t>Senha</t>
+  </si>
+  <si>
+    <t>Primeiro_Nome</t>
+  </si>
+  <si>
+    <t>Ultimo_Nome</t>
+  </si>
+  <si>
+    <t>Telefone</t>
+  </si>
+  <si>
+    <t>Pais</t>
+  </si>
+  <si>
+    <t>Cidade</t>
+  </si>
+  <si>
+    <t>Endereco</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>CEP</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>testepkapjh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +117,13 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -145,9 +152,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -466,7 +474,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,8 +482,8 @@
     <col min="1" max="1" width="12.140625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" customWidth="1"/>
@@ -483,73 +491,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -557,5 +565,6 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{03798983-A7B4-40B6-9896-956CFA47E221}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
criacao das classes LoginLogic, LoginStep, LoginPage, LoginRunner e da feature login.feature
</commit_message>
<xml_diff>
--- a/Usuario_Cadastro.xlsx
+++ b/Usuario_Cadastro.xlsx
@@ -1,113 +1,150 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\eclipse-workspace\advantage-shopping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\KeeggoExercicio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CB0997-2497-4452-A09A-500F8D5D05A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB77017-971C-4D3F-B6FA-65E0A498D6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{B6BE7F0E-3B9E-4F50-8BA9-7697DEB93021}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Usuario" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+  <si>
+    <t>Usuario</t>
+  </si>
   <si>
     <t>Email</t>
   </si>
   <si>
-    <t>gabriel@keeggo.com</t>
-  </si>
-  <si>
-    <t>Gabriel#2022</t>
-  </si>
-  <si>
-    <t>Gabriel</t>
-  </si>
-  <si>
-    <t>Soares</t>
-  </si>
-  <si>
-    <t>2020-2020</t>
+    <t>Senha</t>
+  </si>
+  <si>
+    <t>Primeiro_Nome</t>
+  </si>
+  <si>
+    <t>Ultimo_Nome</t>
+  </si>
+  <si>
+    <t>Telefone</t>
+  </si>
+  <si>
+    <t>Pais</t>
+  </si>
+  <si>
+    <t>Cidade</t>
+  </si>
+  <si>
+    <t>Endereco</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>CEP</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>teste@teste.com</t>
+  </si>
+  <si>
+    <t>Teste@2021</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>1111-1111</t>
   </si>
   <si>
     <t>Brazil</t>
   </si>
   <si>
-    <t>Parana</t>
-  </si>
-  <si>
-    <t>Curitiba</t>
-  </si>
-  <si>
-    <t>Rua Caramuru</t>
-  </si>
-  <si>
-    <t>08130-310</t>
-  </si>
-  <si>
-    <t>Senha</t>
-  </si>
-  <si>
-    <t>Primeiro_Nome</t>
-  </si>
-  <si>
-    <t>Ultimo_Nome</t>
-  </si>
-  <si>
-    <t>Telefone</t>
-  </si>
-  <si>
-    <t>Pais</t>
-  </si>
-  <si>
-    <t>Cidade</t>
-  </si>
-  <si>
-    <t>Endereco</t>
-  </si>
-  <si>
-    <t>Estado</t>
-  </si>
-  <si>
-    <t>CEP</t>
-  </si>
-  <si>
-    <t>Usuario</t>
+    <t>Osasco</t>
+  </si>
+  <si>
+    <t>Rua Teste</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>11111-125</t>
+  </si>
+  <si>
+    <t>Randomtcrrkdfi</t>
+  </si>
+  <si>
+    <t>Randomptkqbjhz</t>
+  </si>
+  <si>
+    <t>Randomygghgvjn</t>
+  </si>
+  <si>
+    <t>Randomjktjoz</t>
+  </si>
+  <si>
+    <t>Randomquzthk</t>
+  </si>
+  <si>
+    <t>Randomtfffdb</t>
+  </si>
+  <si>
+    <t>testemhgkmc</t>
+  </si>
+  <si>
+    <t>testejdxugm</t>
+  </si>
+  <si>
+    <t>testedasjde</t>
+  </si>
+  <si>
+    <t>testesxowwh</t>
+  </si>
+  <si>
+    <t>testemctgjk</t>
+  </si>
+  <si>
+    <t>testeyqdsde</t>
+  </si>
+  <si>
+    <t>testetuoktd</t>
+  </si>
+  <si>
+    <t>testeanqhce</t>
+  </si>
+  <si>
+    <t>testeyemyfo</t>
   </si>
   <si>
     <t>testepkapjh</t>
+  </si>
+  <si>
+    <t>testeilhhtq</t>
+  </si>
+  <si>
+    <t>testesgimkv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,7 +162,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,17 +195,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -470,101 +514,100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5AE4BC-7C38-4770-96F2-8411C5F6E6CC}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>10</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{03798983-A7B4-40B6-9896-956CFA47E221}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{5AB9F60F-3D95-43FB-A345-C130966710DB}"/>
   </hyperlinks>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
inclusao de metodos e steps nas classes LoginPage, LoginLogic, LoginStep e na feature login.feature respectivamente
</commit_message>
<xml_diff>
--- a/Usuario_Cadastro.xlsx
+++ b/Usuario_Cadastro.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\KeeggoExercicio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\eclipse-workspace\advantage-shopping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB77017-971C-4D3F-B6FA-65E0A498D6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD58F5C-EA7C-46BA-BDEB-42A64DAD11F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuario" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Usuario</t>
   </si>
@@ -55,15 +55,9 @@
     <t>CEP</t>
   </si>
   <si>
-    <t>Random</t>
-  </si>
-  <si>
     <t>teste@teste.com</t>
   </si>
   <si>
-    <t>Teste@2021</t>
-  </si>
-  <si>
     <t>Tester</t>
   </si>
   <si>
@@ -85,58 +79,13 @@
     <t>11111-125</t>
   </si>
   <si>
-    <t>Randomtcrrkdfi</t>
-  </si>
-  <si>
-    <t>Randomptkqbjhz</t>
-  </si>
-  <si>
-    <t>Randomygghgvjn</t>
-  </si>
-  <si>
-    <t>Randomjktjoz</t>
-  </si>
-  <si>
-    <t>Randomquzthk</t>
-  </si>
-  <si>
-    <t>Randomtfffdb</t>
-  </si>
-  <si>
-    <t>testemhgkmc</t>
-  </si>
-  <si>
-    <t>testejdxugm</t>
-  </si>
-  <si>
-    <t>testedasjde</t>
-  </si>
-  <si>
-    <t>testesxowwh</t>
-  </si>
-  <si>
-    <t>testemctgjk</t>
-  </si>
-  <si>
-    <t>testeyqdsde</t>
-  </si>
-  <si>
-    <t>testetuoktd</t>
-  </si>
-  <si>
-    <t>testeanqhce</t>
-  </si>
-  <si>
-    <t>testeyemyfo</t>
-  </si>
-  <si>
-    <t>testepkapjh</t>
-  </si>
-  <si>
-    <t>testeilhhtq</t>
-  </si>
-  <si>
     <t>testesgimkv</t>
+  </si>
+  <si>
+    <t>Teste@2022</t>
+  </si>
+  <si>
+    <t>testeemnswd</t>
   </si>
 </sst>
 </file>
@@ -195,11 +144,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -518,7 +468,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,37 +517,37 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
alteracao nas classes GenericLogic, GenericStep, LoginLogic e LoginPage
</commit_message>
<xml_diff>
--- a/Usuario_Cadastro.xlsx
+++ b/Usuario_Cadastro.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Usuario</t>
   </si>
@@ -86,6 +86,24 @@
   </si>
   <si>
     <t>testeemnswd</t>
+  </si>
+  <si>
+    <t>testegzxxwt</t>
+  </si>
+  <si>
+    <t>testefbewkr</t>
+  </si>
+  <si>
+    <t>testewprxbx</t>
+  </si>
+  <si>
+    <t>testetdjkbq</t>
+  </si>
+  <si>
+    <t>testekkulrw</t>
+  </si>
+  <si>
+    <t>testejtytnm</t>
   </si>
 </sst>
 </file>
@@ -517,7 +535,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
correcao do metodo de logout
</commit_message>
<xml_diff>
--- a/Usuario_Cadastro.xlsx
+++ b/Usuario_Cadastro.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Usuario</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>testejtytnm</t>
+  </si>
+  <si>
+    <t>testeubgelo</t>
   </si>
 </sst>
 </file>
@@ -535,7 +538,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>

</xml_diff>